<commit_message>
BST-MPHARM Fees Head Problem Resolved
</commit_message>
<xml_diff>
--- a/SKFGI/Common/Upload/Attendance.xlsx
+++ b/SKFGI/Common/Upload/Attendance.xlsx
@@ -359,7 +359,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -380,7 +380,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>5</v>

</xml_diff>